<commit_message>
ongoing testing work ... HeadersToClaimsMiddleware
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/HeadersToClaims/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/HeadersToClaims/TestJson.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\ScopeProperties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\HeadersToClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E11B4E8-8CE4-486E-BB7F-F62636121611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EC7DE7-C1A1-4E78-AA89-C3F34ADE78C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="1253" yWindow="1140" windowWidth="17992" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>ProjectName</t>
   </si>
@@ -69,40 +69,25 @@
     <t>ScopePropertiesController</t>
   </si>
   <si>
-    <t>Claims</t>
-  </si>
-  <si>
     <t>Headers</t>
   </si>
   <si>
-    <t>header*hdr1=ABC&amp;header*hdr2=DEF</t>
-  </si>
-  <si>
-    <t>claim*role=user&amp;claim*group=456</t>
-  </si>
-  <si>
-    <t>claim*name=jack&amp;claim*role=admin</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>header*hdr1=123&amp;header*X-User=jill</t>
-  </si>
-  <si>
-    <t>X-User=bob</t>
-  </si>
-  <si>
-    <t>{"User":"bob"}</t>
-  </si>
-  <si>
     <t>ScopePropertiesApi</t>
   </si>
   <si>
-    <t>{"User":"jack","name":"jack","role":"admin","Host":"localhost","hdr1":"ABC","hdr2":"DEF","X-HostPath":"localhost"}</t>
-  </si>
-  <si>
-    <t>{"User":"jill","role":"user","group":"456","Host":"localhost","hdr1":"123","X-User":"jill"}</t>
+    <t>header*X-UserScope=ABC&amp;header*X-Role=admin&amp;header*X-User=moe@stooges.org</t>
+  </si>
+  <si>
+    <t>[{"Type":"X-UserScope","Value":"ABC"}]</t>
+  </si>
+  <si>
+    <t>[{"Type":"X-Role","Value":"admin"},{"Type":"X-User","Value":"moe@stooges.org"}]</t>
+  </si>
+  <si>
+    <t>[{"Type":"X-UserScope","Value":"ABC"},{"Type":"X-Role","Value":"admin"},{"Type":"X-User","Value":"moe@stooges.org"}]</t>
   </si>
 </sst>
 </file>
@@ -455,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -498,7 +483,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -513,12 +498,12 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -530,15 +515,15 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -547,18 +532,18 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -570,15 +555,15 @@
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -587,18 +572,18 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -607,73 +592,13 @@
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ongoing testing work ... HeadersToClaimsMiddleware tests now passing
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/HeadersToClaims/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/HeadersToClaims/TestJson.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\HeadersToClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EC7DE7-C1A1-4E78-AA89-C3F34ADE78C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3718529-D5FD-4D97-88AF-B0D345E5C328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1253" yWindow="1140" windowWidth="17992" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,28 +66,28 @@
     <t>Get</t>
   </si>
   <si>
-    <t>ScopePropertiesController</t>
-  </si>
-  <si>
     <t>Headers</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>ScopePropertiesApi</t>
-  </si>
-  <si>
     <t>header*X-UserScope=ABC&amp;header*X-Role=admin&amp;header*X-User=moe@stooges.org</t>
   </si>
   <si>
-    <t>[{"Type":"X-UserScope","Value":"ABC"}]</t>
-  </si>
-  <si>
-    <t>[{"Type":"X-Role","Value":"admin"},{"Type":"X-User","Value":"moe@stooges.org"}]</t>
-  </si>
-  <si>
-    <t>[{"Type":"X-UserScope","Value":"ABC"},{"Type":"X-Role","Value":"admin"},{"Type":"X-User","Value":"moe@stooges.org"}]</t>
+    <t>HeadersToClaimsApi</t>
+  </si>
+  <si>
+    <t>ClaimsController</t>
+  </si>
+  <si>
+    <t>[{"Type":"user_scope","Value":"ABC"}]</t>
+  </si>
+  <si>
+    <t>[{"Type":"name","Value":"moe@stooges.org"},{"Type":"role","Value":"admin"}]</t>
+  </si>
+  <si>
+    <t>[{"Type":"name","Value":"moe@stooges.org"},{"Type":"role","Value":"admin"},{"Type":"user_scope","Value":"ABC"}]</t>
   </si>
 </sst>
 </file>
@@ -448,10 +448,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1328125" style="1"/>
     <col min="6" max="6" width="9.3984375" style="1" customWidth="1"/>
     <col min="7" max="7" width="42.73046875" style="1" customWidth="1"/>
@@ -486,7 +486,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -495,10 +495,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -506,7 +506,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -526,7 +526,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -535,10 +535,10 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -546,7 +546,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -566,19 +566,19 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -586,13 +586,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>

</xml_diff>